<commit_message>
Updated data for 2.13.02
</commit_message>
<xml_diff>
--- a/sample-data-and-templates/tailoring/TailoredControls.xlsx
+++ b/sample-data-and-templates/tailoring/TailoredControls.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dalebingham/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dalebingham/soteria/OpenRMFPro/openrmfpro-automation/sample-data-and-templates/tailoring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CA1799-EE1C-F04B-8DB6-A71D0726F830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90BEEA69-A8F4-404C-9361-7FA0639411D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="39180" windowHeight="21480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8800" yWindow="980" windowWidth="17160" windowHeight="21080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tailored-Controls" sheetId="1" r:id="rId1"/>
@@ -34,21 +34,12 @@
     <t>AC-1</t>
   </si>
   <si>
-    <t>AC-2</t>
-  </si>
-  <si>
     <t>AC-2(1)</t>
   </si>
   <si>
-    <t>AC-2(2)</t>
-  </si>
-  <si>
     <t>AC-2(3)</t>
   </si>
   <si>
-    <t>AC-2(4)</t>
-  </si>
-  <si>
     <t>AC-2(5)</t>
   </si>
   <si>
@@ -73,9 +64,6 @@
     <t>AC-5</t>
   </si>
   <si>
-    <t>AC-6</t>
-  </si>
-  <si>
     <t>AC-6(1)</t>
   </si>
   <si>
@@ -100,9 +88,6 @@
     <t>AC-7</t>
   </si>
   <si>
-    <t>AC-8</t>
-  </si>
-  <si>
     <t>AC-10</t>
   </si>
   <si>
@@ -667,9 +652,6 @@
     <t>MA-4(3)</t>
   </si>
   <si>
-    <t>MA-5</t>
-  </si>
-  <si>
     <t>MA-5(1)</t>
   </si>
   <si>
@@ -679,9 +661,6 @@
     <t>MP-1</t>
   </si>
   <si>
-    <t>MP-2</t>
-  </si>
-  <si>
     <t>MP-3</t>
   </si>
   <si>
@@ -694,9 +673,6 @@
     <t>MP-6</t>
   </si>
   <si>
-    <t>MP-6(1)</t>
-  </si>
-  <si>
     <t>MP-6(2)</t>
   </si>
   <si>
@@ -1223,6 +1199,30 @@
   </si>
   <si>
     <t>SR-11(3)</t>
+  </si>
+  <si>
+    <t>AC-02</t>
+  </si>
+  <si>
+    <t>AC-2 (2)</t>
+  </si>
+  <si>
+    <t>AC-06</t>
+  </si>
+  <si>
+    <t>AC-08</t>
+  </si>
+  <si>
+    <t>MA-05</t>
+  </si>
+  <si>
+    <t>MP-02</t>
+  </si>
+  <si>
+    <t>MP-06 (01)</t>
+  </si>
+  <si>
+    <t>AC-2 (04)</t>
   </si>
 </sst>
 </file>
@@ -1618,7 +1618,7 @@
   <dimension ref="A1:B399"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1649,7 +1649,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>393</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1657,7 +1657,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1665,7 +1665,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>394</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1673,7 +1673,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1681,7 +1681,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>400</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1689,7 +1689,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1697,7 +1697,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1705,7 +1705,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1713,7 +1713,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1721,7 +1721,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1729,7 +1729,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1737,7 +1737,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1745,7 +1745,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1753,7 +1753,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>17</v>
+        <v>395</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1761,7 +1761,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1769,7 +1769,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1777,7 +1777,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1785,7 +1785,7 @@
         <v>2</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1793,7 +1793,7 @@
         <v>2</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1801,7 +1801,7 @@
         <v>2</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1809,7 +1809,7 @@
         <v>2</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1817,7 +1817,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1825,7 +1825,7 @@
         <v>2</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>26</v>
+        <v>396</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1833,7 +1833,7 @@
         <v>2</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1841,7 +1841,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1849,7 +1849,7 @@
         <v>2</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1857,7 +1857,7 @@
         <v>2</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1865,7 +1865,7 @@
         <v>2</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1873,7 +1873,7 @@
         <v>2</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1881,7 +1881,7 @@
         <v>2</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1889,7 +1889,7 @@
         <v>2</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1897,7 +1897,7 @@
         <v>2</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1905,7 +1905,7 @@
         <v>2</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1913,7 +1913,7 @@
         <v>2</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1921,7 +1921,7 @@
         <v>2</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1929,7 +1929,7 @@
         <v>2</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1937,7 +1937,7 @@
         <v>2</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1945,7 +1945,7 @@
         <v>2</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1953,7 +1953,7 @@
         <v>2</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1961,7 +1961,7 @@
         <v>2</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1969,7 +1969,7 @@
         <v>2</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1977,7 +1977,7 @@
         <v>2</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1985,7 +1985,7 @@
         <v>2</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1993,7 +1993,7 @@
         <v>2</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2001,7 +2001,7 @@
         <v>2</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2009,7 +2009,7 @@
         <v>2</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2017,7 +2017,7 @@
         <v>2</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2025,7 +2025,7 @@
         <v>2</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2033,7 +2033,7 @@
         <v>2</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2041,7 +2041,7 @@
         <v>2</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2049,7 +2049,7 @@
         <v>2</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2057,7 +2057,7 @@
         <v>2</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2065,7 +2065,7 @@
         <v>2</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2073,7 +2073,7 @@
         <v>2</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2081,7 +2081,7 @@
         <v>2</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2089,7 +2089,7 @@
         <v>2</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2097,7 +2097,7 @@
         <v>2</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2105,7 +2105,7 @@
         <v>2</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2113,7 +2113,7 @@
         <v>2</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2121,7 +2121,7 @@
         <v>2</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2129,7 +2129,7 @@
         <v>2</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2137,7 +2137,7 @@
         <v>2</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2145,7 +2145,7 @@
         <v>2</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2153,7 +2153,7 @@
         <v>2</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2161,7 +2161,7 @@
         <v>2</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2169,7 +2169,7 @@
         <v>2</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2177,7 +2177,7 @@
         <v>2</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2185,7 +2185,7 @@
         <v>2</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2193,7 +2193,7 @@
         <v>2</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2201,7 +2201,7 @@
         <v>2</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2209,7 +2209,7 @@
         <v>2</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2217,7 +2217,7 @@
         <v>2</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2225,7 +2225,7 @@
         <v>2</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2233,7 +2233,7 @@
         <v>2</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2241,7 +2241,7 @@
         <v>2</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2249,7 +2249,7 @@
         <v>2</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2257,7 +2257,7 @@
         <v>2</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2265,7 +2265,7 @@
         <v>2</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2273,7 +2273,7 @@
         <v>2</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2281,7 +2281,7 @@
         <v>2</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2289,7 +2289,7 @@
         <v>2</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2297,7 +2297,7 @@
         <v>2</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2305,7 +2305,7 @@
         <v>2</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2313,7 +2313,7 @@
         <v>2</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2321,7 +2321,7 @@
         <v>2</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2329,7 +2329,7 @@
         <v>2</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2337,7 +2337,7 @@
         <v>2</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2345,7 +2345,7 @@
         <v>2</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2353,7 +2353,7 @@
         <v>2</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2361,7 +2361,7 @@
         <v>2</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2369,7 +2369,7 @@
         <v>2</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2377,7 +2377,7 @@
         <v>2</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2385,7 +2385,7 @@
         <v>2</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2393,7 +2393,7 @@
         <v>2</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2401,7 +2401,7 @@
         <v>2</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2409,7 +2409,7 @@
         <v>2</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2417,7 +2417,7 @@
         <v>2</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2425,7 +2425,7 @@
         <v>2</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2433,7 +2433,7 @@
         <v>2</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2441,7 +2441,7 @@
         <v>2</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2449,7 +2449,7 @@
         <v>2</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2457,7 +2457,7 @@
         <v>2</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2465,7 +2465,7 @@
         <v>2</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2473,7 +2473,7 @@
         <v>2</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2481,7 +2481,7 @@
         <v>2</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2489,7 +2489,7 @@
         <v>2</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2497,7 +2497,7 @@
         <v>2</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2505,7 +2505,7 @@
         <v>2</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2513,7 +2513,7 @@
         <v>2</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2521,7 +2521,7 @@
         <v>2</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2529,7 +2529,7 @@
         <v>2</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2537,7 +2537,7 @@
         <v>2</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2545,7 +2545,7 @@
         <v>2</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2553,7 +2553,7 @@
         <v>2</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2561,7 +2561,7 @@
         <v>2</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2569,7 +2569,7 @@
         <v>2</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2577,7 +2577,7 @@
         <v>2</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2585,7 +2585,7 @@
         <v>2</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2593,7 +2593,7 @@
         <v>2</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2601,7 +2601,7 @@
         <v>2</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2609,7 +2609,7 @@
         <v>2</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2617,7 +2617,7 @@
         <v>2</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2625,7 +2625,7 @@
         <v>2</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2633,7 +2633,7 @@
         <v>2</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2641,7 +2641,7 @@
         <v>2</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2649,7 +2649,7 @@
         <v>2</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2657,7 +2657,7 @@
         <v>2</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2665,7 +2665,7 @@
         <v>2</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2673,7 +2673,7 @@
         <v>2</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2681,7 +2681,7 @@
         <v>2</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2689,7 +2689,7 @@
         <v>2</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2697,7 +2697,7 @@
         <v>2</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2705,7 +2705,7 @@
         <v>2</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2713,7 +2713,7 @@
         <v>2</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2721,7 +2721,7 @@
         <v>2</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2729,7 +2729,7 @@
         <v>2</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2737,7 +2737,7 @@
         <v>2</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2745,7 +2745,7 @@
         <v>2</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2753,7 +2753,7 @@
         <v>2</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2761,7 +2761,7 @@
         <v>2</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2769,7 +2769,7 @@
         <v>2</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2777,7 +2777,7 @@
         <v>2</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2785,7 +2785,7 @@
         <v>2</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2793,7 +2793,7 @@
         <v>2</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2801,7 +2801,7 @@
         <v>2</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2809,7 +2809,7 @@
         <v>2</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2817,7 +2817,7 @@
         <v>2</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2825,7 +2825,7 @@
         <v>2</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2833,7 +2833,7 @@
         <v>2</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2841,7 +2841,7 @@
         <v>2</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2849,7 +2849,7 @@
         <v>2</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2857,7 +2857,7 @@
         <v>2</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2865,7 +2865,7 @@
         <v>2</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2873,7 +2873,7 @@
         <v>2</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2881,7 +2881,7 @@
         <v>2</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2889,7 +2889,7 @@
         <v>2</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2897,7 +2897,7 @@
         <v>2</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2905,7 +2905,7 @@
         <v>2</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2913,7 +2913,7 @@
         <v>2</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2921,7 +2921,7 @@
         <v>2</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2929,7 +2929,7 @@
         <v>2</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2937,7 +2937,7 @@
         <v>2</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2945,7 +2945,7 @@
         <v>2</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2953,7 +2953,7 @@
         <v>2</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2961,7 +2961,7 @@
         <v>2</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2969,7 +2969,7 @@
         <v>2</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2977,7 +2977,7 @@
         <v>2</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2985,7 +2985,7 @@
         <v>2</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -2993,7 +2993,7 @@
         <v>2</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3001,7 +3001,7 @@
         <v>2</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3009,7 +3009,7 @@
         <v>2</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3017,7 +3017,7 @@
         <v>2</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3025,7 +3025,7 @@
         <v>2</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3033,7 +3033,7 @@
         <v>2</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3041,7 +3041,7 @@
         <v>2</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3049,7 +3049,7 @@
         <v>2</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3057,7 +3057,7 @@
         <v>2</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3065,7 +3065,7 @@
         <v>2</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3073,7 +3073,7 @@
         <v>2</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3081,7 +3081,7 @@
         <v>2</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3089,7 +3089,7 @@
         <v>2</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3097,7 +3097,7 @@
         <v>2</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3105,7 +3105,7 @@
         <v>2</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3113,7 +3113,7 @@
         <v>2</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3121,7 +3121,7 @@
         <v>2</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3129,7 +3129,7 @@
         <v>2</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3137,7 +3137,7 @@
         <v>2</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3145,7 +3145,7 @@
         <v>2</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3153,7 +3153,7 @@
         <v>2</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3161,7 +3161,7 @@
         <v>2</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3169,7 +3169,7 @@
         <v>2</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3177,7 +3177,7 @@
         <v>2</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3185,7 +3185,7 @@
         <v>2</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3193,7 +3193,7 @@
         <v>2</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3201,7 +3201,7 @@
         <v>2</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3209,7 +3209,7 @@
         <v>2</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3217,7 +3217,7 @@
         <v>2</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3225,7 +3225,7 @@
         <v>2</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3233,7 +3233,7 @@
         <v>2</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3241,7 +3241,7 @@
         <v>2</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3249,7 +3249,7 @@
         <v>2</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3257,7 +3257,7 @@
         <v>2</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3265,7 +3265,7 @@
         <v>2</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3273,7 +3273,7 @@
         <v>2</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3281,7 +3281,7 @@
         <v>2</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3289,7 +3289,7 @@
         <v>2</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3297,7 +3297,7 @@
         <v>2</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3305,7 +3305,7 @@
         <v>2</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3313,7 +3313,7 @@
         <v>2</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3321,7 +3321,7 @@
         <v>2</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3329,7 +3329,7 @@
         <v>2</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3337,7 +3337,7 @@
         <v>2</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>215</v>
+        <v>397</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3345,7 +3345,7 @@
         <v>2</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3353,7 +3353,7 @@
         <v>2</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3361,7 +3361,7 @@
         <v>2</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3369,7 +3369,7 @@
         <v>2</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>219</v>
+        <v>398</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3377,7 +3377,7 @@
         <v>2</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3385,7 +3385,7 @@
         <v>2</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3393,7 +3393,7 @@
         <v>2</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3401,7 +3401,7 @@
         <v>2</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3409,7 +3409,7 @@
         <v>2</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>224</v>
+        <v>399</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3417,7 +3417,7 @@
         <v>2</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3425,7 +3425,7 @@
         <v>2</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3433,7 +3433,7 @@
         <v>2</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3441,7 +3441,7 @@
         <v>2</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3449,7 +3449,7 @@
         <v>2</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3457,7 +3457,7 @@
         <v>2</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3465,7 +3465,7 @@
         <v>2</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3473,7 +3473,7 @@
         <v>2</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3481,7 +3481,7 @@
         <v>2</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3489,7 +3489,7 @@
         <v>2</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3497,7 +3497,7 @@
         <v>2</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3505,7 +3505,7 @@
         <v>2</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3513,7 +3513,7 @@
         <v>2</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3521,7 +3521,7 @@
         <v>2</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3529,7 +3529,7 @@
         <v>2</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3537,7 +3537,7 @@
         <v>2</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3545,7 +3545,7 @@
         <v>2</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3553,7 +3553,7 @@
         <v>2</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3561,7 +3561,7 @@
         <v>2</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3569,7 +3569,7 @@
         <v>2</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3577,7 +3577,7 @@
         <v>2</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3585,7 +3585,7 @@
         <v>2</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3593,7 +3593,7 @@
         <v>2</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3601,7 +3601,7 @@
         <v>2</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3609,7 +3609,7 @@
         <v>2</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3617,7 +3617,7 @@
         <v>2</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3625,7 +3625,7 @@
         <v>2</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3633,7 +3633,7 @@
         <v>2</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3641,7 +3641,7 @@
         <v>2</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3649,7 +3649,7 @@
         <v>2</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3657,7 +3657,7 @@
         <v>2</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3665,7 +3665,7 @@
         <v>2</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3673,7 +3673,7 @@
         <v>2</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3681,7 +3681,7 @@
         <v>2</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3689,7 +3689,7 @@
         <v>2</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3697,7 +3697,7 @@
         <v>2</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3705,7 +3705,7 @@
         <v>2</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3713,7 +3713,7 @@
         <v>2</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3721,7 +3721,7 @@
         <v>2</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3729,7 +3729,7 @@
         <v>2</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3737,7 +3737,7 @@
         <v>2</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3745,7 +3745,7 @@
         <v>2</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3753,7 +3753,7 @@
         <v>2</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3761,7 +3761,7 @@
         <v>2</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3769,7 +3769,7 @@
         <v>2</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3777,7 +3777,7 @@
         <v>2</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3785,7 +3785,7 @@
         <v>2</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
     </row>
     <row r="271" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3793,7 +3793,7 @@
         <v>2</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3801,7 +3801,7 @@
         <v>2</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3809,7 +3809,7 @@
         <v>2</v>
       </c>
       <c r="B273" s="2" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
     </row>
     <row r="274" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3817,7 +3817,7 @@
         <v>2</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="275" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3825,7 +3825,7 @@
         <v>2</v>
       </c>
       <c r="B275" s="2" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3833,7 +3833,7 @@
         <v>2</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3841,7 +3841,7 @@
         <v>2</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3849,7 +3849,7 @@
         <v>2</v>
       </c>
       <c r="B278" s="2" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3857,7 +3857,7 @@
         <v>2</v>
       </c>
       <c r="B279" s="2" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3865,7 +3865,7 @@
         <v>2</v>
       </c>
       <c r="B280" s="2" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3873,7 +3873,7 @@
         <v>2</v>
       </c>
       <c r="B281" s="2" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3881,7 +3881,7 @@
         <v>2</v>
       </c>
       <c r="B282" s="2" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3889,7 +3889,7 @@
         <v>2</v>
       </c>
       <c r="B283" s="2" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3897,7 +3897,7 @@
         <v>2</v>
       </c>
       <c r="B284" s="2" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3905,7 +3905,7 @@
         <v>2</v>
       </c>
       <c r="B285" s="2" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3913,7 +3913,7 @@
         <v>2</v>
       </c>
       <c r="B286" s="2" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3921,7 +3921,7 @@
         <v>2</v>
       </c>
       <c r="B287" s="2" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3929,7 +3929,7 @@
         <v>2</v>
       </c>
       <c r="B288" s="2" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3937,7 +3937,7 @@
         <v>2</v>
       </c>
       <c r="B289" s="2" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3945,7 +3945,7 @@
         <v>2</v>
       </c>
       <c r="B290" s="2" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3953,7 +3953,7 @@
         <v>2</v>
       </c>
       <c r="B291" s="2" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3961,7 +3961,7 @@
         <v>2</v>
       </c>
       <c r="B292" s="2" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3969,7 +3969,7 @@
         <v>2</v>
       </c>
       <c r="B293" s="2" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3977,7 +3977,7 @@
         <v>2</v>
       </c>
       <c r="B294" s="2" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3985,7 +3985,7 @@
         <v>2</v>
       </c>
       <c r="B295" s="2" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -3993,7 +3993,7 @@
         <v>2</v>
       </c>
       <c r="B296" s="2" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4001,7 +4001,7 @@
         <v>2</v>
       </c>
       <c r="B297" s="2" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4009,7 +4009,7 @@
         <v>2</v>
       </c>
       <c r="B298" s="2" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4017,7 +4017,7 @@
         <v>2</v>
       </c>
       <c r="B299" s="2" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4025,7 +4025,7 @@
         <v>2</v>
       </c>
       <c r="B300" s="2" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4033,7 +4033,7 @@
         <v>2</v>
       </c>
       <c r="B301" s="2" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
     </row>
     <row r="302" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4041,7 +4041,7 @@
         <v>2</v>
       </c>
       <c r="B302" s="2" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
     </row>
     <row r="303" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4049,7 +4049,7 @@
         <v>2</v>
       </c>
       <c r="B303" s="2" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
     </row>
     <row r="304" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4057,7 +4057,7 @@
         <v>2</v>
       </c>
       <c r="B304" s="2" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
     </row>
     <row r="305" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4065,7 +4065,7 @@
         <v>2</v>
       </c>
       <c r="B305" s="2" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
     </row>
     <row r="306" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4073,7 +4073,7 @@
         <v>2</v>
       </c>
       <c r="B306" s="2" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
     </row>
     <row r="307" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4081,7 +4081,7 @@
         <v>2</v>
       </c>
       <c r="B307" s="2" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
     </row>
     <row r="308" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4089,7 +4089,7 @@
         <v>2</v>
       </c>
       <c r="B308" s="2" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
     </row>
     <row r="309" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4097,7 +4097,7 @@
         <v>2</v>
       </c>
       <c r="B309" s="2" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
     </row>
     <row r="310" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4105,7 +4105,7 @@
         <v>2</v>
       </c>
       <c r="B310" s="2" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
     </row>
     <row r="311" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4113,7 +4113,7 @@
         <v>2</v>
       </c>
       <c r="B311" s="2" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4121,7 +4121,7 @@
         <v>2</v>
       </c>
       <c r="B312" s="2" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4129,7 +4129,7 @@
         <v>2</v>
       </c>
       <c r="B313" s="2" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4137,7 +4137,7 @@
         <v>2</v>
       </c>
       <c r="B314" s="2" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4145,7 +4145,7 @@
         <v>2</v>
       </c>
       <c r="B315" s="2" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4153,7 +4153,7 @@
         <v>2</v>
       </c>
       <c r="B316" s="2" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4161,7 +4161,7 @@
         <v>2</v>
       </c>
       <c r="B317" s="2" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4169,7 +4169,7 @@
         <v>2</v>
       </c>
       <c r="B318" s="2" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4177,7 +4177,7 @@
         <v>2</v>
       </c>
       <c r="B319" s="2" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4185,7 +4185,7 @@
         <v>2</v>
       </c>
       <c r="B320" s="2" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4193,7 +4193,7 @@
         <v>2</v>
       </c>
       <c r="B321" s="2" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4201,7 +4201,7 @@
         <v>2</v>
       </c>
       <c r="B322" s="2" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
     </row>
     <row r="323" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4209,7 +4209,7 @@
         <v>2</v>
       </c>
       <c r="B323" s="2" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
     </row>
     <row r="324" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4217,7 +4217,7 @@
         <v>2</v>
       </c>
       <c r="B324" s="2" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4225,7 +4225,7 @@
         <v>2</v>
       </c>
       <c r="B325" s="2" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4233,7 +4233,7 @@
         <v>2</v>
       </c>
       <c r="B326" s="2" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4241,7 +4241,7 @@
         <v>2</v>
       </c>
       <c r="B327" s="2" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4249,7 +4249,7 @@
         <v>2</v>
       </c>
       <c r="B328" s="2" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4257,7 +4257,7 @@
         <v>2</v>
       </c>
       <c r="B329" s="2" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4265,7 +4265,7 @@
         <v>2</v>
       </c>
       <c r="B330" s="2" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
     </row>
     <row r="331" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4273,7 +4273,7 @@
         <v>2</v>
       </c>
       <c r="B331" s="2" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
     </row>
     <row r="332" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4281,7 +4281,7 @@
         <v>2</v>
       </c>
       <c r="B332" s="2" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4289,7 +4289,7 @@
         <v>2</v>
       </c>
       <c r="B333" s="2" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
     </row>
     <row r="334" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4297,7 +4297,7 @@
         <v>2</v>
       </c>
       <c r="B334" s="2" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4305,7 +4305,7 @@
         <v>2</v>
       </c>
       <c r="B335" s="2" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4313,7 +4313,7 @@
         <v>2</v>
       </c>
       <c r="B336" s="2" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4321,7 +4321,7 @@
         <v>2</v>
       </c>
       <c r="B337" s="2" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4329,7 +4329,7 @@
         <v>2</v>
       </c>
       <c r="B338" s="2" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
     </row>
     <row r="339" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4337,7 +4337,7 @@
         <v>2</v>
       </c>
       <c r="B339" s="2" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
     </row>
     <row r="340" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4345,7 +4345,7 @@
         <v>2</v>
       </c>
       <c r="B340" s="2" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
     </row>
     <row r="341" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4353,7 +4353,7 @@
         <v>2</v>
       </c>
       <c r="B341" s="2" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
     </row>
     <row r="342" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4361,7 +4361,7 @@
         <v>2</v>
       </c>
       <c r="B342" s="2" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
     </row>
     <row r="343" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4369,7 +4369,7 @@
         <v>2</v>
       </c>
       <c r="B343" s="2" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
     </row>
     <row r="344" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4377,7 +4377,7 @@
         <v>2</v>
       </c>
       <c r="B344" s="2" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
     </row>
     <row r="345" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4385,7 +4385,7 @@
         <v>2</v>
       </c>
       <c r="B345" s="2" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
     </row>
     <row r="346" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4393,7 +4393,7 @@
         <v>2</v>
       </c>
       <c r="B346" s="2" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="347" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4401,7 +4401,7 @@
         <v>2</v>
       </c>
       <c r="B347" s="2" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
     </row>
     <row r="348" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4409,7 +4409,7 @@
         <v>2</v>
       </c>
       <c r="B348" s="2" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
     </row>
     <row r="349" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4417,7 +4417,7 @@
         <v>2</v>
       </c>
       <c r="B349" s="2" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
     </row>
     <row r="350" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4425,7 +4425,7 @@
         <v>2</v>
       </c>
       <c r="B350" s="2" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
     </row>
     <row r="351" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4433,7 +4433,7 @@
         <v>2</v>
       </c>
       <c r="B351" s="2" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
     </row>
     <row r="352" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4441,7 +4441,7 @@
         <v>2</v>
       </c>
       <c r="B352" s="2" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
     </row>
     <row r="353" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4449,7 +4449,7 @@
         <v>2</v>
       </c>
       <c r="B353" s="2" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
     </row>
     <row r="354" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4457,7 +4457,7 @@
         <v>2</v>
       </c>
       <c r="B354" s="2" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
     </row>
     <row r="355" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4465,7 +4465,7 @@
         <v>2</v>
       </c>
       <c r="B355" s="2" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
     </row>
     <row r="356" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4473,7 +4473,7 @@
         <v>2</v>
       </c>
       <c r="B356" s="2" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
     </row>
     <row r="357" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4481,7 +4481,7 @@
         <v>2</v>
       </c>
       <c r="B357" s="2" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
     </row>
     <row r="358" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4489,7 +4489,7 @@
         <v>2</v>
       </c>
       <c r="B358" s="2" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
     </row>
     <row r="359" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4497,7 +4497,7 @@
         <v>2</v>
       </c>
       <c r="B359" s="2" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
     </row>
     <row r="360" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4505,7 +4505,7 @@
         <v>2</v>
       </c>
       <c r="B360" s="2" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
     </row>
     <row r="361" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4513,7 +4513,7 @@
         <v>2</v>
       </c>
       <c r="B361" s="2" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4521,7 +4521,7 @@
         <v>2</v>
       </c>
       <c r="B362" s="2" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="363" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4529,7 +4529,7 @@
         <v>2</v>
       </c>
       <c r="B363" s="2" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4537,7 +4537,7 @@
         <v>2</v>
       </c>
       <c r="B364" s="2" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4545,7 +4545,7 @@
         <v>2</v>
       </c>
       <c r="B365" s="2" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4553,7 +4553,7 @@
         <v>2</v>
       </c>
       <c r="B366" s="2" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4561,7 +4561,7 @@
         <v>2</v>
       </c>
       <c r="B367" s="2" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
     </row>
     <row r="368" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4569,7 +4569,7 @@
         <v>2</v>
       </c>
       <c r="B368" s="2" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4577,7 +4577,7 @@
         <v>2</v>
       </c>
       <c r="B369" s="2" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4585,7 +4585,7 @@
         <v>2</v>
       </c>
       <c r="B370" s="2" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4593,7 +4593,7 @@
         <v>2</v>
       </c>
       <c r="B371" s="2" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
     </row>
     <row r="372" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4601,7 +4601,7 @@
         <v>2</v>
       </c>
       <c r="B372" s="2" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4609,7 +4609,7 @@
         <v>2</v>
       </c>
       <c r="B373" s="2" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="374" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4617,7 +4617,7 @@
         <v>2</v>
       </c>
       <c r="B374" s="2" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4625,7 +4625,7 @@
         <v>2</v>
       </c>
       <c r="B375" s="2" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
     </row>
     <row r="376" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4633,7 +4633,7 @@
         <v>2</v>
       </c>
       <c r="B376" s="2" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4641,7 +4641,7 @@
         <v>2</v>
       </c>
       <c r="B377" s="2" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
     </row>
     <row r="378" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4649,7 +4649,7 @@
         <v>2</v>
       </c>
       <c r="B378" s="2" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
     </row>
     <row r="379" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4657,7 +4657,7 @@
         <v>2</v>
       </c>
       <c r="B379" s="2" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
     </row>
     <row r="380" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4665,7 +4665,7 @@
         <v>2</v>
       </c>
       <c r="B380" s="2" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
     </row>
     <row r="381" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4673,7 +4673,7 @@
         <v>2</v>
       </c>
       <c r="B381" s="2" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
     </row>
     <row r="382" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4681,7 +4681,7 @@
         <v>2</v>
       </c>
       <c r="B382" s="2" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
     </row>
     <row r="383" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4689,7 +4689,7 @@
         <v>2</v>
       </c>
       <c r="B383" s="2" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
     </row>
     <row r="384" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4697,7 +4697,7 @@
         <v>2</v>
       </c>
       <c r="B384" s="2" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
     </row>
     <row r="385" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4705,7 +4705,7 @@
         <v>2</v>
       </c>
       <c r="B385" s="2" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
     </row>
     <row r="386" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4713,7 +4713,7 @@
         <v>2</v>
       </c>
       <c r="B386" s="2" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
     </row>
     <row r="387" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4721,7 +4721,7 @@
         <v>2</v>
       </c>
       <c r="B387" s="2" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
     </row>
     <row r="388" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4729,7 +4729,7 @@
         <v>2</v>
       </c>
       <c r="B388" s="2" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
     </row>
     <row r="389" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4737,7 +4737,7 @@
         <v>2</v>
       </c>
       <c r="B389" s="2" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
     </row>
     <row r="390" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4745,7 +4745,7 @@
         <v>2</v>
       </c>
       <c r="B390" s="2" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
     </row>
     <row r="391" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4753,7 +4753,7 @@
         <v>2</v>
       </c>
       <c r="B391" s="2" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
     </row>
     <row r="392" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4761,7 +4761,7 @@
         <v>2</v>
       </c>
       <c r="B392" s="2" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
     </row>
     <row r="393" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4769,7 +4769,7 @@
         <v>2</v>
       </c>
       <c r="B393" s="2" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
     </row>
     <row r="394" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4777,7 +4777,7 @@
         <v>2</v>
       </c>
       <c r="B394" s="2" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
     </row>
     <row r="395" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4785,7 +4785,7 @@
         <v>2</v>
       </c>
       <c r="B395" s="2" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
     </row>
     <row r="396" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4793,7 +4793,7 @@
         <v>2</v>
       </c>
       <c r="B396" s="2" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4801,7 +4801,7 @@
         <v>2</v>
       </c>
       <c r="B397" s="2" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
     </row>
     <row r="398" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4809,7 +4809,7 @@
         <v>2</v>
       </c>
       <c r="B398" s="2" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
     </row>
     <row r="399" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -4817,7 +4817,7 @@
         <v>2</v>
       </c>
       <c r="B399" s="2" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
   </sheetData>

</xml_diff>